<commit_message>
fixed one outlier in LWC live oaks
</commit_message>
<xml_diff>
--- a/data/pv_curves/PV_curves.xlsx
+++ b/data/pv_curves/PV_curves.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Desktop/github/SHIFT/data/pv_curves/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5378F1-DF47-6645-A264-145FD6FDB5F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A7C5CA-5471-D94A-BF1C-AE614215ADB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="760" windowWidth="25640" windowHeight="16020" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="760" windowWidth="25640" windowHeight="16020" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2382" sheetId="24" r:id="rId1"/>
@@ -12452,8 +12452,8 @@
   </sheetPr>
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView zoomScale="113" zoomScaleNormal="105" zoomScalePageLayoutView="105" workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="105" zoomScalePageLayoutView="105" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14258,7 +14258,7 @@
   </sheetPr>
   <dimension ref="A1:Q102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>

</xml_diff>